<commit_message>
Second version of PCB with more peripheral devices
</commit_message>
<xml_diff>
--- a/Four-leg robot/Project Outputs for Four-leg robot/Four-leg robot bom.xlsx
+++ b/Four-leg robot/Project Outputs for Four-leg robot/Four-leg robot bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamil\Desktop\TUL\Semestr VII\praca inżynierska\PCB\Four-leg robot\Project Outputs for Four-leg robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DE5C193-5FF0-4177-9CD6-F9822A86AFA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A8E8CE-E643-46F4-A45A-4BEC76EA6499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-9585" windowWidth="29040" windowHeight="15840" xr2:uid="{3A9319FC-91C4-4007-8F37-7F3012595EF3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="141">
   <si>
     <t>Comment</t>
   </si>
@@ -326,9 +326,6 @@
     <t>DE1209-22 Coil</t>
   </si>
   <si>
-    <t>https://www.tme.eu/pl/details/dtsm31n/mikroprzelaczniki-tact/diptronics/</t>
-  </si>
-  <si>
     <t>Bluetooth</t>
   </si>
   <si>
@@ -377,9 +374,6 @@
     <t>C3, C4, C5, C6, C7, C8, C9, C10, C11, C12</t>
   </si>
   <si>
-    <t>https://www.tme.eu/pl/details/t821-1-10-s1/zlacza-idc/amphenol/t821110a1s100ceu/</t>
-  </si>
-  <si>
     <t>https://www.tme.eu/pl/details/16.00m-hc49-s/rezonatory-kwarcowe-tht/yic/</t>
   </si>
   <si>
@@ -453,13 +447,22 @@
   </si>
   <si>
     <t>min. 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/pl/details/zl231-10pg/zlacza-idc/connfly/ds1013-10ssib1/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/pl/details/dtsm31n-f/mikroprzelaczniki-tact/ninigi/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,8 +504,18 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <strike/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,6 +543,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -582,7 +601,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -590,7 +609,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -602,9 +620,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -920,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A05A25-7435-48A2-9F57-F5A5DCC81541}">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,11 +992,11 @@
       <c r="J1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>131</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -997,8 +1018,8 @@
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>105</v>
+      <c r="G2" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="H2">
         <v>0.62960000000000005</v>
@@ -1020,16 +1041,16 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
         <v>107</v>
       </c>
-      <c r="B3" t="s">
-        <v>108</v>
-      </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>106</v>
+      <c r="G3" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="H3">
         <v>1.7878000000000001</v>
@@ -1057,10 +1078,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
@@ -1068,8 +1089,8 @@
       <c r="F4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>112</v>
+      <c r="G4" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="H4">
         <v>3.95</v>
@@ -1091,122 +1112,122 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>109</v>
+        <v>2</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="H5">
-        <v>0.29119</v>
+        <v>0.90654999999999997</v>
       </c>
       <c r="I5">
-        <v>0.35799999999999998</v>
+        <v>1.1160000000000001</v>
       </c>
       <c r="J5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
-        <v>2.9119000000000002</v>
+        <f>IF($J5&gt;$F5,H5*$J5,H5*$F5)</f>
+        <v>4.5327500000000001</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
-        <v>3.58</v>
+        <f>IF($J5&gt;$F5,I5*$J5,I5*$F5)</f>
+        <v>5.58</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="F6" s="3">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>117</v>
+        <v>1</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="H6">
-        <v>0.90654999999999997</v>
+        <v>3.17</v>
       </c>
       <c r="I6">
-        <v>1.1160000000000001</v>
+        <v>3.9</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>4.5327500000000001</v>
+        <f>IF($J6&gt;$F6,H6*$J6,H6*$F6)</f>
+        <v>3.17</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
-        <v>5.58</v>
+        <f>IF($J6&gt;$F6,I6*$J6,I6*$F6)</f>
+        <v>3.9</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="F7" s="3">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>116</v>
+        <v>2</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="H7">
-        <v>0.51763999999999999</v>
+        <v>0.63570000000000004</v>
       </c>
       <c r="I7">
-        <v>0.63700000000000001</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="J7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
-        <v>5.1764000000000001</v>
+        <f>IF($J7&gt;$F7,H7*$J7,H7*$F7)</f>
+        <v>3.1785000000000001</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
-        <v>6.37</v>
+        <f>IF($J7&gt;$F7,I7*$J7,I7*$F7)</f>
+        <v>3.91</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1228,7 +1249,7 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="19" t="s">
         <v>87</v>
       </c>
       <c r="H8">
@@ -1268,25 +1289,25 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
-        <v>114</v>
+      <c r="G9" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="H9">
-        <v>1.7881</v>
+        <v>0.3</v>
       </c>
       <c r="I9">
-        <v>2.21</v>
+        <v>0.5</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>3.5762</v>
+        <v>3</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>4.42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1308,7 +1329,7 @@
       <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="7" t="s">
         <v>95</v>
       </c>
       <c r="H10">
@@ -1348,8 +1369,8 @@
       <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>135</v>
+      <c r="G11" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="H11">
         <v>1.6839999999999999</v>
@@ -1369,611 +1390,637 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="O11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="F12" s="3">
-        <v>3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>124</v>
+        <v>9</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="H12">
-        <v>0.63570000000000004</v>
+        <v>3.882E-2</v>
       </c>
       <c r="I12">
-        <v>0.78200000000000003</v>
+        <v>4.7699999999999999E-2</v>
       </c>
       <c r="J12">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
-        <v>3.1785000000000001</v>
+        <f>IF($J12&gt;$F12,H12*$J12,H12*$F12)</f>
+        <v>3.8820000000000001</v>
       </c>
       <c r="L12">
-        <f t="shared" si="0"/>
-        <v>3.91</v>
+        <f>IF($J12&gt;$F12,I12*$J12,I12*$F12)</f>
+        <v>4.7699999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F13" s="3">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>91</v>
+        <v>2</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>140</v>
       </c>
       <c r="H13">
-        <v>3.17</v>
+        <v>0.84460000000000002</v>
       </c>
       <c r="I13">
-        <v>3.9</v>
+        <v>0.45476</v>
       </c>
       <c r="J13">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
-        <v>3.17</v>
+        <f>IF($J13&gt;$F13,H13*$J13,H13*$F13)</f>
+        <v>8.4459999999999997</v>
       </c>
       <c r="L13">
-        <f t="shared" si="0"/>
-        <v>3.9</v>
+        <f>IF($J13&gt;$F13,I13*$J13,I13*$F13)</f>
+        <v>4.5476000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="I14">
+        <v>5.35</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f>IF($J14&gt;$F14,H14*$J14,H14*$F14)</f>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="L14">
+        <f>IF($J14&gt;$F14,I14*$J14,I14*$F14)</f>
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="5">
+        <v>10.19</v>
+      </c>
+      <c r="I15">
+        <v>12.53</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <f>IF($J15&gt;$F15,H15*$J15,H15*$F15)</f>
+        <v>10.19</v>
+      </c>
+      <c r="L15">
+        <f>IF($J15&gt;$F15,I15*$J15,I15*$F15)</f>
+        <v>12.53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="3">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>104</v>
-      </c>
-      <c r="H14">
-        <v>0.63570000000000004</v>
-      </c>
-      <c r="I14">
-        <v>0.78200000000000003</v>
-      </c>
-      <c r="J14">
-        <v>2</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>1.2714000000000001</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="0"/>
-        <v>1.5640000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>126</v>
-      </c>
-      <c r="H15">
-        <v>5.5199999999999999E-2</v>
-      </c>
-      <c r="I15">
-        <v>6.9699999999999998E-2</v>
-      </c>
-      <c r="J15">
-        <v>100</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>5.52</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="0"/>
-        <v>6.97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F16" s="4">
-        <v>3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>125</v>
+      <c r="E16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="H16">
-        <v>5.5199999999999999E-2</v>
+        <v>2.99</v>
       </c>
       <c r="I16">
-        <v>6.7900000000000002E-2</v>
+        <v>3.68</v>
       </c>
       <c r="J16">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="K16">
-        <f t="shared" si="0"/>
-        <v>5.52</v>
+        <f>IF($J16&gt;$F16,H16*$J16,H16*$F16)</f>
+        <v>2.99</v>
       </c>
       <c r="L16">
-        <f t="shared" si="0"/>
-        <v>6.79</v>
+        <f>IF($J16&gt;$F16,I16*$J16,I16*$F16)</f>
+        <v>3.68</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17">
+        <v>2.3401999999999998</v>
+      </c>
+      <c r="I17">
+        <v>2.87</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <f>IF($J17&gt;$F17,H17*$J17,H17*$F17)</f>
+        <v>4.6803999999999997</v>
+      </c>
+      <c r="L17">
+        <f>IF($J17&gt;$F17,I17*$J17,I17*$F17)</f>
+        <v>5.74</v>
+      </c>
+      <c r="O17" t="s">
+        <v>136</v>
+      </c>
+      <c r="P17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13">
+        <f>SUM(K2:K17)</f>
+        <v>72.121250000000003</v>
+      </c>
+      <c r="L21" s="13">
+        <f>SUM(L2:L17)</f>
+        <v>84.167600000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="17">
+        <v>1</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" s="18">
+        <v>25.1</v>
+      </c>
+      <c r="I25" s="18">
+        <v>25.1</v>
+      </c>
+      <c r="J25" s="18">
+        <v>1</v>
+      </c>
+      <c r="K25" s="18">
+        <f>IF($J25&gt;$F25,H25*$J25,H25*$F25)</f>
+        <v>25.1</v>
+      </c>
+      <c r="L25" s="18">
+        <f>IF($J25&gt;$F25,I25*$J25,I25*$F25)</f>
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="9">
+        <v>1</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H29" s="6">
+        <v>0.29119</v>
+      </c>
+      <c r="I29" s="6">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="J29" s="6">
+        <v>10</v>
+      </c>
+      <c r="K29" s="6">
+        <f>IF($J29&gt;$F29,H29*$J29,H29*$F29)</f>
+        <v>2.9119000000000002</v>
+      </c>
+      <c r="L29" s="6">
+        <f>IF($J29&gt;$F29,I29*$J29,I29*$F29)</f>
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="9">
+        <v>10</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" s="6">
+        <v>0.51763999999999999</v>
+      </c>
+      <c r="I30" s="6">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="J30" s="6">
+        <v>10</v>
+      </c>
+      <c r="K30" s="6">
+        <f>IF($J30&gt;$F30,H30*$J30,H30*$F30)</f>
+        <v>5.1764000000000001</v>
+      </c>
+      <c r="L30" s="6">
+        <f>IF($J30&gt;$F30,I30*$J30,I30*$F30)</f>
+        <v>6.37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="9">
+        <v>3</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H31" s="6">
+        <v>0.63570000000000004</v>
+      </c>
+      <c r="I31" s="6">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="J31" s="6">
+        <v>5</v>
+      </c>
+      <c r="K31" s="6">
+        <f>IF($J31&gt;$F31,H31*$J31,H31*$F31)</f>
+        <v>3.1785000000000001</v>
+      </c>
+      <c r="L31" s="6">
+        <f>IF($J31&gt;$F31,I31*$J31,I31*$F31)</f>
+        <v>3.91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="9">
+        <v>1</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H32" s="6">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="I32" s="6">
+        <f>8.37+(23%*H32)</f>
+        <v>10.2951</v>
+      </c>
+      <c r="J32" s="6">
+        <v>1</v>
+      </c>
+      <c r="K32" s="6">
+        <f>IF($J32&gt;$F32,H32*$J32,H32*$F32)</f>
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="L32" s="6">
+        <f>IF($J32&gt;$F32,I32*$J32,I32*$F32)</f>
+        <v>10.2951</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C33" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="9">
+        <v>1</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H33" s="6">
+        <v>5.5199999999999999E-2</v>
+      </c>
+      <c r="I33" s="6">
+        <v>6.9699999999999998E-2</v>
+      </c>
+      <c r="J33" s="6">
+        <v>100</v>
+      </c>
+      <c r="K33" s="6">
+        <f>IF($J33&gt;$F33,H33*$J33,H33*$F33)</f>
+        <v>5.52</v>
+      </c>
+      <c r="L33" s="6">
+        <f>IF($J33&gt;$F33,I33*$J33,I33*$F33)</f>
+        <v>6.97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="15">
+        <v>3</v>
+      </c>
+      <c r="G34" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="3">
-        <v>9</v>
-      </c>
-      <c r="G17" t="s">
-        <v>128</v>
-      </c>
-      <c r="H17">
-        <v>3.882E-2</v>
-      </c>
-      <c r="I17">
-        <v>4.7699999999999999E-2</v>
-      </c>
-      <c r="J17">
+      <c r="H34" s="6">
+        <v>5.5199999999999999E-2</v>
+      </c>
+      <c r="I34" s="6">
+        <v>6.7900000000000002E-2</v>
+      </c>
+      <c r="J34" s="6">
         <v>100</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>3.8820000000000001</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="0"/>
-        <v>4.7699999999999996</v>
-      </c>
-      <c r="O17" t="s">
-        <v>138</v>
-      </c>
-      <c r="P17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="K34" s="6">
+        <f>IF($J34&gt;$F34,H34*$J34,H34*$F34)</f>
+        <v>5.52</v>
+      </c>
+      <c r="L34" s="6">
+        <f>IF($J34&gt;$F34,I34*$J34,I34*$F34)</f>
+        <v>6.79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="11">
         <v>2</v>
       </c>
-      <c r="G18" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18">
-        <v>0.84460000000000002</v>
-      </c>
-      <c r="I18">
-        <v>1.04</v>
-      </c>
-      <c r="J18">
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="9">
+        <v>12</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H39" s="6">
+        <v>0.6502</v>
+      </c>
+      <c r="I39" s="6">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="J39" s="6">
         <v>5</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>4.2229999999999999</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="0"/>
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="H19">
-        <v>8.3699999999999992</v>
-      </c>
-      <c r="I19">
-        <f>8.37+(23%*H19)</f>
-        <v>10.2951</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>8.3699999999999992</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="0"/>
-        <v>10.2951</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>94</v>
-      </c>
-      <c r="H20">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="I20">
-        <v>5.35</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="0"/>
-        <v>5.35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="3">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>86</v>
-      </c>
-      <c r="H21" s="6">
-        <v>10.19</v>
-      </c>
-      <c r="I21">
-        <v>12.53</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
-        <v>10.19</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="0"/>
-        <v>12.53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22">
-        <v>2.99</v>
-      </c>
-      <c r="I22">
-        <v>3.68</v>
-      </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="0"/>
-        <v>2.99</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="0"/>
-        <v>3.68</v>
-      </c>
-      <c r="O22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
-        <v>115</v>
-      </c>
-      <c r="H23">
-        <v>2.3401999999999998</v>
-      </c>
-      <c r="I23">
-        <v>2.87</v>
-      </c>
-      <c r="J23">
-        <v>2</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="0"/>
-        <v>4.6803999999999997</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="0"/>
-        <v>5.74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F24" s="4">
-        <v>1</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="H24">
-        <v>25.1</v>
-      </c>
-      <c r="I24">
-        <v>25.1</v>
-      </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="0"/>
-        <v>25.1</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="0"/>
-        <v>25.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" s="12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F27" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F28" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" s="10">
-        <v>12</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="H29" s="7">
-        <v>0.6502</v>
-      </c>
-      <c r="I29" s="7">
-        <v>0.80400000000000005</v>
-      </c>
-      <c r="J29" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14">
-        <f>SUM(K2:K24)</f>
-        <v>122.34415000000001</v>
-      </c>
-      <c r="L31" s="14">
-        <f>SUM(L2:L24)</f>
-        <v>144.9091</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{D62AE30A-D89F-40EC-9243-F0378E7625CA}"/>
     <hyperlink ref="G11" r:id="rId2" xr:uid="{81F793C7-18E4-4AE1-9A9E-91DFBA041C70}"/>
+    <hyperlink ref="G32" r:id="rId3" xr:uid="{4445FBA5-FB6D-4630-BBD2-B587867C1169}"/>
+    <hyperlink ref="G15" r:id="rId4" xr:uid="{62A16650-537C-4755-877D-7E2C0570D851}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{62811BB1-842E-4847-A0F8-5DAD15B32A71}"/>
+    <hyperlink ref="G2" r:id="rId6" xr:uid="{A2AA4745-12F4-4F68-8A8D-DC2157454FEC}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{06699140-787C-4E51-9951-FA0DD85ECD7B}"/>
+    <hyperlink ref="G6" r:id="rId8" xr:uid="{A30583A1-A67C-4407-8D9E-E5AADFC9EB3F}"/>
+    <hyperlink ref="G7" r:id="rId9" xr:uid="{F48AE707-2BEA-4497-8823-0FCA8F3B38FC}"/>
+    <hyperlink ref="G8" r:id="rId10" xr:uid="{42FFDB3B-CF2E-4E3E-A2C9-BC1EF2B30BAF}"/>
+    <hyperlink ref="G9" r:id="rId11" xr:uid="{D59B5754-6B2C-425F-BA38-9B1A5AD1967F}"/>
+    <hyperlink ref="G10" r:id="rId12" xr:uid="{BAB5C823-132A-4D5B-987E-E897F29285E1}"/>
+    <hyperlink ref="G12" r:id="rId13" xr:uid="{307D2E73-3A99-4F9B-95C1-5BCF0B006564}"/>
+    <hyperlink ref="G13" r:id="rId14" xr:uid="{169003FA-B067-4A9A-B420-339E0A837EB7}"/>
+    <hyperlink ref="G14" r:id="rId15" xr:uid="{C128F04B-DF5F-41B1-837D-E04736EDA82A}"/>
+    <hyperlink ref="G16" r:id="rId16" xr:uid="{C50F4870-06CD-4000-A392-5F470E47F65C}"/>
+    <hyperlink ref="G17" r:id="rId17" xr:uid="{EC2E3BFD-F29B-4CE0-8C69-A4E62A46B0C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>